<commit_message>
added more functionality to the document forms objects so that i can modify attributes to trigger document load. This allows modification of documents. Converted to modal popup style for nicer UX concider creating an extension. TODO: there is an issue with base query element as documented in journal
</commit_message>
<xml_diff>
--- a/Planning Report/application sprint planner sprint1 11.11.19 - Copy.xlsx
+++ b/Planning Report/application sprint planner sprint1 11.11.19 - Copy.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0DB766-B12A-4CC2-9284-169F3A7FBCD5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A63A6C-49BD-403D-BC16-29BA82C4729D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="855" yWindow="0" windowWidth="22275" windowHeight="15600" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="11" r:id="rId1"/>
@@ -1313,6 +1313,40 @@
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
   </cellStyles>
   <dxfs count="92">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -2818,40 +2852,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border>
         <left style="thin">
           <color theme="0" tint="-0.24994659260841701"/>
@@ -3173,10 +3173,10 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Milestone description" dataDxfId="79"/>
-    <tableColumn id="7" xr3:uid="{C2AA6DD8-DBD1-4E89-A1EF-3287225D3E74}" name="Required" dataDxfId="78"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Category" dataDxfId="77"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Estimated Duration" dataDxfId="76"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Milestone description" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{C2AA6DD8-DBD1-4E89-A1EF-3287225D3E74}" name="Required" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Category" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Estimated Duration" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Start" dataCellStyle="Date"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="No. Days" dataCellStyle="Comma [0]"/>
@@ -3457,7 +3457,7 @@
   <dimension ref="A1:BM83"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5123,9 +5123,15 @@
       <c r="E13" s="34">
         <v>4</v>
       </c>
-      <c r="F13" s="31"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="33"/>
+      <c r="F13" s="31">
+        <v>1</v>
+      </c>
+      <c r="G13" s="32">
+        <v>43781</v>
+      </c>
+      <c r="H13" s="33">
+        <v>1</v>
+      </c>
       <c r="I13" s="26"/>
       <c r="J13" s="38"/>
       <c r="K13" s="38"/>
@@ -19242,56 +19248,56 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:BM8 J80:BM81 J52:BM55 J61:BM61 J37:BM37 J58:BM58 J67:BM67 J47:BM50 J39:BM40 J10:BM10 J22:BM25 J27:BM34">
-    <cfRule type="expression" dxfId="75" priority="243">
+    <cfRule type="expression" dxfId="79" priority="243">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:AN4">
-    <cfRule type="expression" dxfId="74" priority="249">
+    <cfRule type="expression" dxfId="78" priority="249">
       <formula>J$5&lt;=EOMONTH($J$5,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:BM4">
-    <cfRule type="expression" dxfId="73" priority="245">
+    <cfRule type="expression" dxfId="77" priority="245">
       <formula>AND(K$5&lt;=EOMONTH($J$5,2),K$5&gt;EOMONTH($J$5,0),K$5&gt;EOMONTH($J$5,1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:BM4">
-    <cfRule type="expression" dxfId="72" priority="244">
+    <cfRule type="expression" dxfId="76" priority="244">
       <formula>AND(J$5&lt;=EOMONTH($J$5,1),J$5&gt;EOMONTH($J$5,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:BM8 J10:BM10 J22:BM80">
-    <cfRule type="expression" dxfId="71" priority="266" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="266" stopIfTrue="1">
       <formula>AND($D8="Low risk",J$5&gt;=$G8,J$5&lt;=$G8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="285" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="285" stopIfTrue="1">
       <formula>AND($D8="High risk",J$5&gt;=$G8,J$5&lt;=$G8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="303" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="303" stopIfTrue="1">
       <formula>AND($D8="On track",J$5&gt;=$G8,J$5&lt;=$G8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="304" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="304" stopIfTrue="1">
       <formula>AND($D8="Med risk",J$5&gt;=$G8,J$5&lt;=$G8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="305" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="305" stopIfTrue="1">
       <formula>AND(LEN($D8)=0,J$5&gt;=$G8,J$5&lt;=$G8+$H8-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J81:BM81">
-    <cfRule type="expression" dxfId="66" priority="313" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="313" stopIfTrue="1">
       <formula>AND(#REF!="Low risk",J$5&gt;=#REF!,J$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="314" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="314" stopIfTrue="1">
       <formula>AND(#REF!="High risk",J$5&gt;=#REF!,J$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="315" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="315" stopIfTrue="1">
       <formula>AND(#REF!="On track",J$5&gt;=#REF!,J$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="316" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="316" stopIfTrue="1">
       <formula>AND(#REF!="Med risk",J$5&gt;=#REF!,J$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="317" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="317" stopIfTrue="1">
       <formula>AND(LEN(#REF!)=0,J$5&gt;=#REF!,J$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19310,24 +19316,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:BM9">
-    <cfRule type="expression" dxfId="61" priority="234">
+    <cfRule type="expression" dxfId="65" priority="234">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:BM9">
-    <cfRule type="expression" dxfId="60" priority="236" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="236" stopIfTrue="1">
       <formula>AND($D9="Low risk",J$5&gt;=$G9,J$5&lt;=$G9+$H9-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="237" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="237" stopIfTrue="1">
       <formula>AND($D9="High risk",J$5&gt;=$G9,J$5&lt;=$G9+$H9-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="238" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="238" stopIfTrue="1">
       <formula>AND($D9="On track",J$5&gt;=$G9,J$5&lt;=$G9+$H9-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="239" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="239" stopIfTrue="1">
       <formula>AND($D9="Med risk",J$5&gt;=$G9,J$5&lt;=$G9+$H9-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="240" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="240" stopIfTrue="1">
       <formula>AND(LEN($D9)=0,J$5&gt;=$G9,J$5&lt;=$G9+$H9-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19346,7 +19352,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J44:BM44 J41:BM42">
-    <cfRule type="expression" dxfId="55" priority="218">
+    <cfRule type="expression" dxfId="59" priority="218">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19365,7 +19371,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J46:GC46">
-    <cfRule type="expression" dxfId="54" priority="209">
+    <cfRule type="expression" dxfId="58" priority="209">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19384,7 +19390,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J45:BM45 J43:BM43">
-    <cfRule type="expression" dxfId="53" priority="202">
+    <cfRule type="expression" dxfId="57" priority="202">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19403,7 +19409,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J26:BM26">
-    <cfRule type="expression" dxfId="52" priority="194">
+    <cfRule type="expression" dxfId="56" priority="194">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19422,7 +19428,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J51:GC51">
-    <cfRule type="expression" dxfId="51" priority="185">
+    <cfRule type="expression" dxfId="55" priority="185">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19441,7 +19447,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J62:GC63 J65:GC67 J70:GC70 J77:GC79">
-    <cfRule type="expression" dxfId="50" priority="178">
+    <cfRule type="expression" dxfId="54" priority="178">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19460,7 +19466,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J64:GC64">
-    <cfRule type="expression" dxfId="49" priority="170">
+    <cfRule type="expression" dxfId="53" priority="170">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19479,7 +19485,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J60:GC60">
-    <cfRule type="expression" dxfId="48" priority="161">
+    <cfRule type="expression" dxfId="52" priority="161">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19498,7 +19504,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J36:GC36">
-    <cfRule type="expression" dxfId="47" priority="153">
+    <cfRule type="expression" dxfId="51" priority="153">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19517,7 +19523,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J57:BM57">
-    <cfRule type="expression" dxfId="46" priority="145">
+    <cfRule type="expression" dxfId="50" priority="145">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19536,7 +19542,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J68:GC69">
-    <cfRule type="expression" dxfId="45" priority="137">
+    <cfRule type="expression" dxfId="49" priority="137">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19555,7 +19561,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J71:GC72">
-    <cfRule type="expression" dxfId="44" priority="129">
+    <cfRule type="expression" dxfId="48" priority="129">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19574,7 +19580,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J75:GC75">
-    <cfRule type="expression" dxfId="43" priority="121">
+    <cfRule type="expression" dxfId="47" priority="121">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19593,7 +19599,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J76:GC76">
-    <cfRule type="expression" dxfId="42" priority="113">
+    <cfRule type="expression" dxfId="46" priority="113">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19612,7 +19618,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J59:BM59">
-    <cfRule type="expression" dxfId="41" priority="105">
+    <cfRule type="expression" dxfId="45" priority="105">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19631,7 +19637,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J38:BM38">
-    <cfRule type="expression" dxfId="40" priority="97">
+    <cfRule type="expression" dxfId="44" priority="97">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19650,7 +19656,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J74:BM74">
-    <cfRule type="expression" dxfId="39" priority="89">
+    <cfRule type="expression" dxfId="43" priority="89">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19669,7 +19675,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J56:BM56">
-    <cfRule type="expression" dxfId="38" priority="57">
+    <cfRule type="expression" dxfId="42" priority="57">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19688,12 +19694,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J73:GC73">
-    <cfRule type="expression" dxfId="37" priority="65">
+    <cfRule type="expression" dxfId="41" priority="65">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J35:BM35">
-    <cfRule type="expression" dxfId="36" priority="49">
+    <cfRule type="expression" dxfId="40" priority="49">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19726,24 +19732,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:BM11">
-    <cfRule type="expression" dxfId="35" priority="41">
+    <cfRule type="expression" dxfId="39" priority="41">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:BM11">
-    <cfRule type="expression" dxfId="34" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="43" stopIfTrue="1">
       <formula>AND($D11="Low risk",J$5&gt;=$G11,J$5&lt;=$G11+$H11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="44" stopIfTrue="1">
       <formula>AND($D11="High risk",J$5&gt;=$G11,J$5&lt;=$G11+$H11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="45" stopIfTrue="1">
       <formula>AND($D11="On track",J$5&gt;=$G11,J$5&lt;=$G11+$H11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="46" stopIfTrue="1">
       <formula>AND($D11="Med risk",J$5&gt;=$G11,J$5&lt;=$G11+$H11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="47" stopIfTrue="1">
       <formula>AND(LEN($D11)=0,J$5&gt;=$G11,J$5&lt;=$G11+$H11-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19762,24 +19768,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:BM14">
-    <cfRule type="expression" dxfId="29" priority="33">
+    <cfRule type="expression" dxfId="33" priority="33">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:BM14">
-    <cfRule type="expression" dxfId="28" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="35" stopIfTrue="1">
       <formula>AND($D12="Low risk",J$5&gt;=$G12,J$5&lt;=$G12+$H12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="36" stopIfTrue="1">
       <formula>AND($D12="High risk",J$5&gt;=$G12,J$5&lt;=$G12+$H12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="37" stopIfTrue="1">
       <formula>AND($D12="On track",J$5&gt;=$G12,J$5&lt;=$G12+$H12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="38" stopIfTrue="1">
       <formula>AND($D12="Med risk",J$5&gt;=$G12,J$5&lt;=$G12+$H12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="39" stopIfTrue="1">
       <formula>AND(LEN($D12)=0,J$5&gt;=$G12,J$5&lt;=$G12+$H12-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19798,24 +19804,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:BM15">
-    <cfRule type="expression" dxfId="23" priority="25">
+    <cfRule type="expression" dxfId="27" priority="25">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:BM15">
-    <cfRule type="expression" dxfId="22" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="27" stopIfTrue="1">
       <formula>AND($D15="Low risk",J$5&gt;=$G15,J$5&lt;=$G15+$H15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="28" stopIfTrue="1">
       <formula>AND($D15="High risk",J$5&gt;=$G15,J$5&lt;=$G15+$H15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="29" stopIfTrue="1">
       <formula>AND($D15="On track",J$5&gt;=$G15,J$5&lt;=$G15+$H15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="30" stopIfTrue="1">
       <formula>AND($D15="Med risk",J$5&gt;=$G15,J$5&lt;=$G15+$H15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="31" stopIfTrue="1">
       <formula>AND(LEN($D15)=0,J$5&gt;=$G15,J$5&lt;=$G15+$H15-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19834,46 +19840,46 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:BM18">
-    <cfRule type="expression" dxfId="17" priority="17">
+    <cfRule type="expression" dxfId="21" priority="17">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:BM18">
-    <cfRule type="expression" dxfId="16" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="19" stopIfTrue="1">
       <formula>AND($D16="Low risk",J$5&gt;=$G16,J$5&lt;=$G16+$H16-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="20" stopIfTrue="1">
       <formula>AND($D16="High risk",J$5&gt;=$G16,J$5&lt;=$G16+$H16-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="21" stopIfTrue="1">
       <formula>AND($D16="On track",J$5&gt;=$G16,J$5&lt;=$G16+$H16-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="22" stopIfTrue="1">
       <formula>AND($D16="Med risk",J$5&gt;=$G16,J$5&lt;=$G16+$H16-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="23" stopIfTrue="1">
       <formula>AND(LEN($D16)=0,J$5&gt;=$G16,J$5&lt;=$G16+$H16-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19:BM19">
-    <cfRule type="expression" dxfId="11" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="12" stopIfTrue="1">
       <formula>AND($D19="Low risk",J$5&gt;=$G19,J$5&lt;=$G19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="13" stopIfTrue="1">
       <formula>AND($D19="High risk",J$5&gt;=$G19,J$5&lt;=$G19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="14" stopIfTrue="1">
       <formula>AND($D19="On track",J$5&gt;=$G19,J$5&lt;=$G19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="15" stopIfTrue="1">
       <formula>AND($D19="Med risk",J$5&gt;=$G19,J$5&lt;=$G19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="16" stopIfTrue="1">
       <formula>AND(LEN($D19)=0,J$5&gt;=$G19,J$5&lt;=$G19+$H19-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19:BM19">
-    <cfRule type="expression" dxfId="6" priority="9">
+    <cfRule type="expression" dxfId="10" priority="9">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19892,19 +19898,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20:BM21">
-    <cfRule type="expression" dxfId="5" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="4" stopIfTrue="1">
       <formula>AND($D20="Low risk",J$5&gt;=$G20,J$5&lt;=$G20+$H20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="5" stopIfTrue="1">
       <formula>AND($D20="High risk",J$5&gt;=$G20,J$5&lt;=$G20+$H20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="6" stopIfTrue="1">
       <formula>AND($D20="On track",J$5&gt;=$G20,J$5&lt;=$G20+$H20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
       <formula>AND($D20="Med risk",J$5&gt;=$G20,J$5&lt;=$G20+$H20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="8" stopIfTrue="1">
       <formula>AND(LEN($D20)=0,J$5&gt;=$G20,J$5&lt;=$G20+$H20-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19923,7 +19929,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20:GC21">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>